<commit_message>
ajout fichiers pour fitting
</commit_message>
<xml_diff>
--- a/Data for fitting en h.xlsx
+++ b/Data for fitting en h.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\process-development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\composting code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E70F6C-991F-4711-A84D-04C8A7744435}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57511465-923B-449A-9F11-9722F52F6EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="5" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Composition of waste" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="651">
   <si>
     <t>Valeurs</t>
   </si>
@@ -1986,6 +1986,15 @@
   </si>
   <si>
     <t>TF on Slg</t>
+  </si>
+  <si>
+    <t>r44</t>
+  </si>
+  <si>
+    <t>Xa on NH4+</t>
+  </si>
+  <si>
+    <t>Y(X/NO3-)</t>
   </si>
 </sst>
 </file>
@@ -2373,8 +2382,8 @@
       <sheetName val="reg"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="14">
           <cell r="L14">
@@ -2404,6 +2413,16 @@
             <v>247</v>
           </cell>
         </row>
+        <row r="20">
+          <cell r="L20">
+            <v>113</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="L21">
+            <v>113</v>
+          </cell>
+        </row>
         <row r="22">
           <cell r="L22">
             <v>18</v>
@@ -2421,6 +2440,11 @@
         </row>
         <row r="25">
           <cell r="L25">
+            <v>62</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="L26">
             <v>17</v>
           </cell>
         </row>
@@ -2471,12 +2495,32 @@
             <v>0.51862348178137652</v>
           </cell>
         </row>
+        <row r="13">
+          <cell r="B13">
+            <v>1.83</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>2.1000000000000001E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>1.0409999999999999</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>0.98</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -26117,7 +26161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DF1B96-6F36-403A-A03F-B41BA123E54D}">
   <dimension ref="A1:CD106"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
@@ -50585,8 +50629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51411,6 +51455,22 @@
       </c>
       <c r="E20" s="2" t="s">
         <v>310</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -51937,13 +51997,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E22A85-0A6D-4692-91B9-50CA4D04329A}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.36328125" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.54296875" style="23" bestFit="1" customWidth="1"/>
@@ -53401,10 +53461,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEDA152-43C0-431A-9CB7-AED9414AC560}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53425,6 +53485,9 @@
       <c r="F1" t="s">
         <v>598</v>
       </c>
+      <c r="G1" t="s">
+        <v>650</v>
+      </c>
       <c r="H1" t="s">
         <v>599</v>
       </c>
@@ -53441,7 +53504,7 @@
         <v>0.61286157024793375</v>
       </c>
       <c r="D2">
-        <f>([1]Variables!M14/[1]Variables!L25)</f>
+        <f>([1]Variables!M14/[1]Variables!L26)</f>
         <v>0.70588235294117652</v>
       </c>
       <c r="E2">
@@ -53468,7 +53531,7 @@
         <v>0.34845814977973566</v>
       </c>
       <c r="D3">
-        <f>([1]Variables!L14/[1]Variables!L25)*([1]stoe!B4/(4-[1]stoe!B4))</f>
+        <f>([1]Variables!L14/[1]Variables!L26)*([1]stoe!B4/(4-[1]stoe!B4))</f>
         <v>2.4906254472591955</v>
       </c>
       <c r="E3">
@@ -53495,7 +53558,7 @@
         <v>0.15679878540876441</v>
       </c>
       <c r="D4">
-        <f>([1]Variables!L14/[1]Variables!L25)</f>
+        <f>([1]Variables!L14/[1]Variables!L26)</f>
         <v>6.6470588235294121</v>
       </c>
       <c r="E4">
@@ -53522,7 +53585,7 @@
         <v>0.61286157024793375</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:G5" si="0">D2</f>
+        <f t="shared" ref="D5:F5" si="0">D2</f>
         <v>0.70588235294117652</v>
       </c>
       <c r="E5">
@@ -53684,7 +53747,7 @@
         <v>0.19196328081035452</v>
       </c>
       <c r="D11">
-        <f>([1]Variables!L16/[1]Variables!L25)</f>
+        <f>([1]Variables!L16/[1]Variables!L26)</f>
         <v>6.6470588235294121</v>
       </c>
       <c r="E11">
@@ -53819,7 +53882,7 @@
         <v>0.59266453382084072</v>
       </c>
       <c r="D16">
-        <f>([1]Variables!L18/[1]Variables!L25)</f>
+        <f>([1]Variables!L18/[1]Variables!L26)</f>
         <v>14.529411764705882</v>
       </c>
       <c r="E16">
@@ -53834,7 +53897,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>630</v>
       </c>
@@ -53846,7 +53909,7 @@
         <v>0.34183471727955711</v>
       </c>
       <c r="D17">
-        <f>([1]Variables!L18/[1]Variables!L25)*([1]stoe!B8/(4-[1]stoe!B8))</f>
+        <f>([1]Variables!L18/[1]Variables!L26)*([1]stoe!B8/(4-[1]stoe!B8))</f>
         <v>2.0698699461283123</v>
       </c>
       <c r="E17">
@@ -53861,7 +53924,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>632</v>
       </c>
@@ -53873,7 +53936,7 @@
         <v>0.14872079850398687</v>
       </c>
       <c r="D18">
-        <f>([1]Variables!L18/[1]Variables!L25)</f>
+        <f>([1]Variables!L18/[1]Variables!L26)</f>
         <v>14.529411764705882</v>
       </c>
       <c r="E18">
@@ -53888,7 +53951,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>634</v>
       </c>
@@ -53900,7 +53963,7 @@
         <v>0.18993587130957534</v>
       </c>
       <c r="D19">
-        <f>[1]Variables!L19/[1]Variables!L25</f>
+        <f>[1]Variables!L19/[1]Variables!L26</f>
         <v>14.529411764705882</v>
       </c>
       <c r="E19">
@@ -53915,7 +53978,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>636</v>
       </c>
@@ -53927,7 +53990,7 @@
         <v>0.21008868149029522</v>
       </c>
       <c r="D20">
-        <f>([1]Variables!L19/[1]Variables!L25)</f>
+        <f>([1]Variables!L19/[1]Variables!L26)</f>
         <v>14.529411764705882</v>
       </c>
       <c r="E20">
@@ -53942,7 +54005,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>638</v>
       </c>
@@ -53969,7 +54032,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>640</v>
       </c>
@@ -53996,7 +54059,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>642</v>
       </c>
@@ -54022,8 +54085,12 @@
       <c r="H23" t="s">
         <v>643</v>
       </c>
+      <c r="J23">
+        <f>(0.021/0.98)*(113/62)</f>
+        <v>3.9055299539170509E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>644</v>
       </c>
@@ -54050,7 +54117,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>646</v>
       </c>
@@ -54075,6 +54142,29 @@
       </c>
       <c r="H25" t="s">
         <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>648</v>
+      </c>
+      <c r="B26">
+        <v>0.13</v>
+      </c>
+      <c r="C26">
+        <f>([1]stoe!B15/[1]stoe!B13)*([1]Variables!L21/[1]Variables!L23)</f>
+        <v>4.0522540983606553E-2</v>
+      </c>
+      <c r="F26">
+        <f>([1]stoe!B15/[1]stoe!B16)*([1]Variables!L20/[1]Variables!L22)</f>
+        <v>0.1266410502721742</v>
+      </c>
+      <c r="G26">
+        <f>([1]stoe!B15/[1]stoe!B17)*([1]Variables!L20/[1]Variables!L25)</f>
+        <v>3.9055299539170509E-2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -54087,7 +54177,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>